<commit_message>
Modified entire example project as per release ac-core version 1.0.1
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rameshwar\Autognizant\ac-projects\ac-example-project\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67827C7F-5504-4C79-9C96-3B4AF3351940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A33ECF9-AC3C-43E1-98C1-0C9A31E1EFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="850"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="@ACAUTO-Scenario3" sheetId="45" r:id="rId1"/>
+    <sheet name="@ACAUTO-Scenario3" sheetId="46" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,8 +64,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,11 +83,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -131,14 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,29 +572,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6153D3-6565-44BA-81B4-3A3BE8361956}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="11.54296875" style="6"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -608,10 +599,10 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -619,10 +610,10 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -637,32 +628,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>